<commit_message>
commit a basic project framework
</commit_message>
<xml_diff>
--- a/tests/words.xlsx
+++ b/tests/words.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaiduSyncdisk\mycode\wordlist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BaiduSyncdisk\mycode\wordlist\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE441C8-BBF6-4534-B534-95D201D18483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB654C2-558B-4E1C-B3C4-EA7B63AA6A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="words" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>单词</t>
   </si>
@@ -56,15 +56,6 @@
   </si>
   <si>
     <t>assemble</t>
-  </si>
-  <si>
-    <t>[əˈsemb(ə)l]</t>
-  </si>
-  <si>
-    <t>v. （使）集合，（使）聚集；装配，组装</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> There wasn't even a convenient place for students to assemble between classes. </t>
   </si>
   <si>
     <t xml:space="preserve"> ...the current batch of trainee priests. </t>
@@ -480,19 +471,19 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="67.26953125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="113.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.06640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.06640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="113.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.53125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -509,9 +500,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="20.25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -526,9 +517,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>9</v>
@@ -537,25 +528,19 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="20.25" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>

</xml_diff>